<commit_message>
ENH/BLD: Implement build, edit, render, check routines with templating and temporary environments for testing
</commit_message>
<xml_diff>
--- a/inst/templates/template_cover_data.xlsx
+++ b/inst/templates/template_cover_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewbain/Documents/career/resume/R/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewbain/Documents/career/resume/inst/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35016E95-C368-FC4C-8800-0FC7784C8900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC747EF-79CA-604F-98AB-7EB78E78B0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="89">
   <si>
     <t>include</t>
   </si>
@@ -77,39 +77,15 @@
     <t>text</t>
   </si>
   <si>
-    <t>industy_experience_aside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have worked in a variety of roles ranging from journalist to software engineer to data scientist. I like collaborative environments where I can learn from my peers. </t>
-  </si>
-  <si>
-    <t>teaching_experience_aside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I am passionate about education. I believe that no topic is too complex if the teacher is empathetic and willing to think about new methods of approaching task. </t>
-  </si>
-  <si>
-    <t>data_science_writing_aside</t>
-  </si>
-  <si>
-    <t>I regularly blog about data science and visualization on my blog [LiveFreeOrDichotomize.](https://livefreeordichotomize.com/)</t>
-  </si>
-  <si>
     <t>word_limit</t>
   </si>
   <si>
     <t>word_count</t>
   </si>
   <si>
-    <t>bainmatt@outlook.com</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>Matthew Bain</t>
-  </si>
-  <si>
     <t>The actual value written for the entry</t>
   </si>
   <si>
@@ -119,18 +95,12 @@
     <t>phone</t>
   </si>
   <si>
-    <t>(647) 567-2509</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
     <t>map-marked-alt</t>
   </si>
   <si>
-    <t>Mississauga, ON</t>
-  </si>
-  <si>
     <t>Calculated field</t>
   </si>
   <si>
@@ -143,102 +113,30 @@
     <t>cover_body</t>
   </si>
   <si>
-    <t>cover_summary</t>
-  </si>
-  <si>
-    <t>cover_achievement_1</t>
-  </si>
-  <si>
-    <t>cover_achievement_2</t>
-  </si>
-  <si>
-    <t>cover_achievement_3</t>
-  </si>
-  <si>
     <t>bio_experience</t>
   </si>
   <si>
     <t>bio_value</t>
   </si>
   <si>
-    <t>My research background, together with my grasp of tricky mathematical theory, allows me to make judicious use of modern methods in Bayesian analysis and natural language processing.</t>
-  </si>
-  <si>
-    <t>Data Analyst and Machine Learning Practitioner</t>
-  </si>
-  <si>
     <t>order</t>
   </si>
   <si>
-    <t>Currently seeking a data science role in which I can apply an object-oriented approach to analytics, visualization, and machine learning development.</t>
-  </si>
-  <si>
-    <t>My experience equips me with strong data management skills, supported by an excellent understanding of statistical theory, as well as excellent programming skills. I am familiar with modern machine learning workflows, pipeline development, and software development best practices. I am also an adept learner, always building my skills in the area further. My adaptability is highlighted by my accelerated completion of a bachelor's degree in mathematics and statistics while actively contributing to the field.</t>
-  </si>
-  <si>
-    <t>cover_preamble</t>
-  </si>
-  <si>
     <t>cover_postscript</t>
   </si>
   <si>
     <t>pic</t>
   </si>
   <si>
-    <t>Note: Title and bio should be shared across resume, LinkedIn, Github, and website</t>
-  </si>
-  <si>
-    <t>In each of my professional and academic roles, I have led initiatives with a shared goal of discovering meaningful patterns in data.</t>
-  </si>
-  <si>
-    <t>I am a highly motivated analyst with 4+ years of experience across academia and industry leveraging data and advanced statistical models to extract value from data.</t>
-  </si>
-  <si>
-    <t>&lt;point 1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;point 2&gt;</t>
-  </si>
-  <si>
-    <t>&lt;point 3&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&gt;</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
-    <t>/Users/matthewbain/Documents/career/headshots/edited/cv_pic.png</t>
-  </si>
-  <si>
     <t>The hyperlink for the entry</t>
   </si>
   <si>
     <t>address_text</t>
   </si>
   <si>
-    <t>tel:+16475672509</t>
-  </si>
-  <si>
-    <t>https://bainmatt.github.io</t>
-  </si>
-  <si>
-    <t>https://github.com/bainmatt</t>
-  </si>
-  <si>
-    <t>https://linkedin.com/in/bainmatt</t>
-  </si>
-  <si>
-    <t>mailto:bainmatt@outlook.com</t>
-  </si>
-  <si>
-    <t>Spanning neuroscience and assistive tech, the central theme of my work is a commitment to building robust and interpretable machine learning systems, helping people understand their data and automate the hard stuff.</t>
-  </si>
-  <si>
-    <t>MSc</t>
-  </si>
-  <si>
     <t>Personal Website</t>
   </si>
   <si>
@@ -246,13 +144,175 @@
   </si>
   <si>
     <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Note: Title and bio should be consistent across resume, LinkedIn, Github, and website</t>
+  </si>
+  <si>
+    <t>cover_opening</t>
+  </si>
+  <si>
+    <t>cover_closing</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>notes/outtakes</t>
+  </si>
+  <si>
+    <t>Dear Hiring Manager,</t>
+  </si>
+  <si>
+    <t>Sincerely,</t>
+  </si>
+  <si>
+    <t>email_subject</t>
+  </si>
+  <si>
+    <t>Application for &lt;position&gt; - &lt;name&gt;</t>
+  </si>
+  <si>
+    <t>concise option</t>
+  </si>
+  <si>
+    <t>I hope this email finds you well. I am writing to express my interest in the &lt;position&gt; position at &lt;company&gt;, as advertised on &lt;where you found the job posting&gt;. Please find attached my resume and cover letter for your review.</t>
+  </si>
+  <si>
+    <t>email_opening</t>
+  </si>
+  <si>
+    <t>email_body</t>
+  </si>
+  <si>
+    <t>email_closing</t>
+  </si>
+  <si>
+    <t>email_postscript</t>
+  </si>
+  <si>
+    <t>alternate option</t>
+  </si>
+  <si>
+    <t>salutation</t>
+  </si>
+  <si>
+    <t>signoff</t>
+  </si>
+  <si>
+    <t>achievement_3</t>
+  </si>
+  <si>
+    <t>achievement_2</t>
+  </si>
+  <si>
+    <t>achievement_1</t>
+  </si>
+  <si>
+    <t>achievements_preamble</t>
+  </si>
+  <si>
+    <t>PhD</t>
+  </si>
+  <si>
+    <t>/absolute/path/to/pic.png</t>
+  </si>
+  <si>
+    <t>City, ST</t>
+  </si>
+  <si>
+    <t>myemail@outlook.com</t>
+  </si>
+  <si>
+    <t>My Name</t>
+  </si>
+  <si>
+    <t>mailto:myemail@outlook.com</t>
+  </si>
+  <si>
+    <t>(999) 999-9999</t>
+  </si>
+  <si>
+    <t>tel:+19999999999</t>
+  </si>
+  <si>
+    <t>https://mysite.com</t>
+  </si>
+  <si>
+    <t>https://github.com/myname</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/myname/</t>
+  </si>
+  <si>
+    <t>This is my experience statement.</t>
+  </si>
+  <si>
+    <t>This is my expertise statement.</t>
+  </si>
+  <si>
+    <t>This is my value statement.</t>
+  </si>
+  <si>
+    <t>My Title</t>
+  </si>
+  <si>
+    <t>This is my objective statement.</t>
+  </si>
+  <si>
+    <t>This is the opening paragraph of my cover letter.</t>
+  </si>
+  <si>
+    <t>This is the body paragraph of my cover letter.</t>
+  </si>
+  <si>
+    <t>This is the closing paragraph of my cover letter.</t>
+  </si>
+  <si>
+    <t>This is a concise version of the opening paragraph of my cover letter.</t>
+  </si>
+  <si>
+    <t>This is a concise version of the body paragraph of my cover letter.</t>
+  </si>
+  <si>
+    <t>This is a concise version of the closing paragraph of my cover letter.</t>
+  </si>
+  <si>
+    <t>Thank you for your consideration. I look forward to the possibility of discussing how my skills and experiences make me a strong fit for the &lt;position&gt; position at &lt;company&gt;.</t>
+  </si>
+  <si>
+    <t>This is a concise version of the postscript of my cover letter.</t>
+  </si>
+  <si>
+    <t>This is the closing paragraph of my email to a recruiter.</t>
+  </si>
+  <si>
+    <t>This is the body text of my email to a recruiter.</t>
+  </si>
+  <si>
+    <t>This statement precedes a set of bullet points highlighting some achievements that make me suitable for the role:</t>
+  </si>
+  <si>
+    <t>This is a description of my first achievement.</t>
+  </si>
+  <si>
+    <t>This is a description of my second achievement.</t>
+  </si>
+  <si>
+    <t>This is a description of my third achievement.</t>
+  </si>
+  <si>
+    <t>This is an alternative option to the above.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -415,9 +475,16 @@
       <family val="2"/>
     </font>
     <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -764,7 +831,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -796,23 +863,26 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -860,13 +930,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1184,7 +1259,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -1196,16 +1271,16 @@
     <col min="6" max="16384" width="10.75" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="3"/>
       <c r="C1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1213,30 +1288,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>3</v>
@@ -1253,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>3</v>
@@ -1261,7 +1336,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
@@ -1270,24 +1345,24 @@
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>3</v>
@@ -1304,27 +1379,27 @@
         <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B8" s="8">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1338,10 +1413,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1355,10 +1430,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1372,10 +1447,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1468,7 @@
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{3DBD8F31-8EF0-694A-BB02-C1527E5FF416}"/>
+    <hyperlink ref="D7" r:id="rId1" display="bainmatt@outlook.com" xr:uid="{3DBD8F31-8EF0-694A-BB02-C1527E5FF416}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1402,376 +1477,755 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC783910-3F85-4C49-B1DE-86999ACD48B8}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="70" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="39.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.25" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="186.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.75" style="5"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="85.75" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="10.75" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="3"/>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" s="5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="E3" s="9">
+        <v>15</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F27" si="0">LEN(TRIM(C3)) - LEN(SUBSTITUTE(C3, " ", "")) + 1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4" si="1">LEN(TRIM(C4)) - LEN(SUBSTITUTE(C4, " ", "")) + 1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>15</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5" si="2">LEN(TRIM(C5)) - LEN(SUBSTITUTE(C5, " ", "")) + 1</f>
+        <v>5</v>
+      </c>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="8">
         <v>3</v>
       </c>
-      <c r="D3" s="8">
+      <c r="E6" s="9">
         <v>15</v>
       </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E3:E17" si="0">LEN(TRIM(F3)) - LEN(SUBSTITUTE(F3, " ", "")) + 1</f>
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="F6" s="9">
+        <f t="shared" ref="F6" si="3">LEN(TRIM(C6)) - LEN(SUBSTITUTE(C6, " ", "")) + 1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="8">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9">
+        <v>15</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" ref="F7" si="4">LEN(TRIM(C7)) - LEN(SUBSTITUTE(C7, " ", "")) + 1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="b">
+      <c r="E8" s="9">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9">
+        <f>LEN(TRIM(C8)) - LEN(SUBSTITUTE(C8, " ", "")) + 1</f>
         <v>1</v>
       </c>
-      <c r="D4" s="8">
-        <v>20</v>
-      </c>
-      <c r="E4" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="8">
+    </row>
+    <row r="9" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>20</v>
-      </c>
-      <c r="E5" s="9">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
+      <c r="E9" s="9">
+        <v>15</v>
+      </c>
+      <c r="F9" s="9">
+        <f>LEN(TRIM(C9)) - LEN(SUBSTITUTE(C9, " ", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="8">
+      <c r="D10" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8">
-        <v>20</v>
-      </c>
-      <c r="E6" s="9">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="E10" s="9">
+        <v>15</v>
+      </c>
+      <c r="F10" s="9">
+        <f>LEN(TRIM(C10)) - LEN(SUBSTITUTE(C10, " ", "")) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8">
         <v>4</v>
       </c>
-      <c r="C7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>20</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8">
-        <v>28</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="E11" s="9">
+        <v>15</v>
+      </c>
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G11" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9">
+        <v>150</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>150</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="9">
+        <v>150</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4</v>
+      </c>
+      <c r="E15" s="9">
+        <v>30</v>
+      </c>
+      <c r="F15" s="9">
+        <f>LEN(TRIM(C15)) - LEN(SUBSTITUTE(C15, " ", "")) + 1</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>150</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16" si="5">LEN(TRIM(C16)) - LEN(SUBSTITUTE(C16, " ", "")) + 1</f>
+        <v>13</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>150</v>
+      </c>
+      <c r="F17" s="9">
+        <f>LEN(TRIM(C17)) - LEN(SUBSTITUTE(C17, " ", "")) + 1</f>
+        <v>13</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="200" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="8">
+        <v>3</v>
+      </c>
+      <c r="E18" s="9">
+        <v>150</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" ref="F18" si="6">LEN(TRIM(C18)) - LEN(SUBSTITUTE(C18, " ", "")) + 1</f>
+        <v>13</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="8">
+        <v>4</v>
+      </c>
+      <c r="E19" s="9">
+        <v>30</v>
+      </c>
+      <c r="F19" s="9">
+        <f>LEN(TRIM(C19)) - LEN(SUBSTITUTE(C19, " ", "")) + 1</f>
+        <v>12</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9">
+        <v>150</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" ref="F20" si="7">LEN(TRIM(C20)) - LEN(SUBSTITUTE(C20, " ", "")) + 1</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2</v>
+      </c>
+      <c r="E21" s="9">
+        <v>150</v>
+      </c>
+      <c r="F21" s="9">
+        <f>LEN(TRIM(C21)) - LEN(SUBSTITUTE(C21, " ", "")) + 1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="8">
+        <v>3</v>
+      </c>
+      <c r="E22" s="9">
+        <v>150</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22" si="8">LEN(TRIM(C22)) - LEN(SUBSTITUTE(C22, " ", "")) + 1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="8">
+        <v>4</v>
+      </c>
+      <c r="E23" s="9">
+        <v>30</v>
+      </c>
+      <c r="F23" s="9">
+        <f>LEN(TRIM(C23)) - LEN(SUBSTITUTE(C23, " ", "")) + 1</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="9">
+        <v>30</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>30</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2</v>
+      </c>
+      <c r="E26" s="9">
+        <v>30</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="B27" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="E27" s="9">
+        <v>30</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="8">
-        <v>50</v>
-      </c>
-      <c r="E9" s="9">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="8">
-        <v>4</v>
-      </c>
-      <c r="C10" s="13" t="b">
+      <c r="E28" s="9">
+        <v>30</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" ref="F28" si="9">LEN(TRIM(C28)) - LEN(SUBSTITUTE(C28, " ", "")) + 1</f>
+        <v>8</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="8">
         <v>1</v>
       </c>
-      <c r="D10" s="8">
-        <v>28</v>
-      </c>
-      <c r="E10" s="9">
-        <f t="shared" si="0"/>
+      <c r="E29" s="9">
+        <v>30</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" ref="F29:F31" si="10">LEN(TRIM(C29)) - LEN(SUBSTITUTE(C29, " ", "")) + 1</f>
+        <v>8</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E30" s="9">
+        <v>30</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="G30" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="8">
+    <row r="31" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="8">
+        <v>3</v>
+      </c>
+      <c r="E31" s="9">
+        <v>30</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="13" t="b">
+      <c r="F32" s="9">
+        <f>LEN(TRIM(C32)) - LEN(SUBSTITUTE(C32, " ", "")) + 1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="9">
+        <v>5</v>
+      </c>
+      <c r="F33" s="9">
+        <f>LEN(TRIM(C33)) - LEN(SUBSTITUTE(C33, " ", "")) + 1</f>
         <v>1</v>
       </c>
-      <c r="D11" s="8">
-        <v>28</v>
-      </c>
-      <c r="E11" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="8">
-        <v>6</v>
-      </c>
-      <c r="C12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
-        <v>28</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="8" t="s">
+    </row>
+    <row r="34" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="8">
-        <v>50</v>
-      </c>
-      <c r="E13" s="9">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="8">
-        <v>28</v>
-      </c>
-      <c r="E14" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="9">
-        <v>28</v>
-      </c>
-      <c r="E15" s="9">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="9">
-        <v>28</v>
-      </c>
-      <c r="E16" s="9">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="9">
-        <v>28</v>
-      </c>
-      <c r="E17" s="9">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="E34" s="9">
+        <v>10</v>
+      </c>
+      <c r="F34" s="9">
+        <f>LEN(TRIM(C34)) - LEN(SUBSTITUTE(C34, " ", "")) + 1</f>
+        <v>5</v>
+      </c>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="56" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="17"/>
+    </row>
+    <row r="59" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="17"/>
+    </row>
+    <row r="64" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F2" xr:uid="{DC783910-3F85-4C49-B1DE-86999ACD48B8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F17">
-      <sortCondition ref="B2:B17"/>
-    </sortState>
-  </autoFilter>
   <customSheetViews>
     <customSheetView guid="{3062D464-6811-D443-AF95-27507DF48802}" showGridLines="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -1780,9 +2234,14 @@
       <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F3:F1012">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($E3 &gt; $D3, NOT(ISBLANK($F3)))</formula>
+  <conditionalFormatting sqref="C3:C100">
+    <cfRule type="expression" dxfId="1" priority="17">
+      <formula>AND($F3 &gt; $E3, NOT(ISBLANK($C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:G100">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>$B3="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>